<commit_message>
Add summary info in excels for read/write distribution.
</commit_message>
<xml_diff>
--- a/example/default_r_latency.xlsx
+++ b/example/default_r_latency.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="181">
   <si>
     <t>ID</t>
   </si>
@@ -31,162 +31,84 @@
     <t>[0~20)</t>
   </si>
   <si>
-    <t>5.59%</t>
-  </si>
-  <si>
     <t>[20~40)</t>
   </si>
   <si>
-    <t>3.14%</t>
-  </si>
-  <si>
     <t>[40~60)</t>
   </si>
   <si>
-    <t>0.46%</t>
-  </si>
-  <si>
     <t>[60~80)</t>
   </si>
   <si>
-    <t>0.36%</t>
-  </si>
-  <si>
     <t>[80~100)</t>
   </si>
   <si>
-    <t>0.04%</t>
-  </si>
-  <si>
     <t>[100~120)</t>
   </si>
   <si>
-    <t>5.95%</t>
-  </si>
-  <si>
     <t>[120~140)</t>
   </si>
   <si>
-    <t>14.03%</t>
-  </si>
-  <si>
     <t>[140~160)</t>
   </si>
   <si>
-    <t>2.38%</t>
-  </si>
-  <si>
     <t>[160~180)</t>
   </si>
   <si>
-    <t>4.75%</t>
-  </si>
-  <si>
     <t>[180~200)</t>
   </si>
   <si>
-    <t>5.57%</t>
-  </si>
-  <si>
     <t>[200~220)</t>
   </si>
   <si>
-    <t>7.57%</t>
-  </si>
-  <si>
     <t>[220~240)</t>
   </si>
   <si>
-    <t>11.58%</t>
-  </si>
-  <si>
     <t>[240~260)</t>
   </si>
   <si>
-    <t>7.05%</t>
-  </si>
-  <si>
     <t>[260~280)</t>
   </si>
   <si>
-    <t>3.04%</t>
-  </si>
-  <si>
     <t>[280~300)</t>
   </si>
   <si>
-    <t>1.67%</t>
-  </si>
-  <si>
     <t>[300~320)</t>
   </si>
   <si>
-    <t>1.22%</t>
-  </si>
-  <si>
     <t>[320~340)</t>
   </si>
   <si>
-    <t>1.37%</t>
-  </si>
-  <si>
     <t>[340~360)</t>
   </si>
   <si>
-    <t>0.89%</t>
-  </si>
-  <si>
     <t>[360~380)</t>
   </si>
   <si>
-    <t>1.79%</t>
-  </si>
-  <si>
     <t>[380~400)</t>
   </si>
   <si>
-    <t>2.51%</t>
-  </si>
-  <si>
     <t>[400~420)</t>
   </si>
   <si>
-    <t>2.53%</t>
-  </si>
-  <si>
     <t>[420~440)</t>
   </si>
   <si>
-    <t>1.03%</t>
-  </si>
-  <si>
     <t>[440~460)</t>
   </si>
   <si>
-    <t>0.27%</t>
-  </si>
-  <si>
     <t>[460~480)</t>
   </si>
   <si>
-    <t>0.21%</t>
-  </si>
-  <si>
     <t>[480~500)</t>
   </si>
   <si>
-    <t>0.55%</t>
-  </si>
-  <si>
     <t>[500~520)</t>
   </si>
   <si>
     <t>[520~540)</t>
   </si>
   <si>
-    <t>0.17%</t>
-  </si>
-  <si>
     <t>[540~560)</t>
   </si>
   <si>
@@ -196,9 +118,6 @@
     <t>[580~600)</t>
   </si>
   <si>
-    <t>0.34%</t>
-  </si>
-  <si>
     <t>[600~620)</t>
   </si>
   <si>
@@ -211,27 +130,15 @@
     <t>[660~680)</t>
   </si>
   <si>
-    <t>0.11%</t>
-  </si>
-  <si>
     <t>[680~700)</t>
   </si>
   <si>
-    <t>0.42%</t>
-  </si>
-  <si>
     <t>[700~720)</t>
   </si>
   <si>
-    <t>0.08%</t>
-  </si>
-  <si>
     <t>[720~740)</t>
   </si>
   <si>
-    <t>0.06%</t>
-  </si>
-  <si>
     <t>[740~760)</t>
   </si>
   <si>
@@ -241,9 +148,6 @@
     <t>[780~800)</t>
   </si>
   <si>
-    <t>0.44%</t>
-  </si>
-  <si>
     <t>[800~820)</t>
   </si>
   <si>
@@ -265,9 +169,6 @@
     <t>[920~940)</t>
   </si>
   <si>
-    <t>0.13%</t>
-  </si>
-  <si>
     <t>[940~960)</t>
   </si>
   <si>
@@ -292,15 +193,9 @@
     <t>[1080~1100)</t>
   </si>
   <si>
-    <t>0.02%</t>
-  </si>
-  <si>
     <t>[1100~1120)</t>
   </si>
   <si>
-    <t>0.25%</t>
-  </si>
-  <si>
     <t>[1120~1140)</t>
   </si>
   <si>
@@ -337,9 +232,6 @@
     <t>[1340~1360)</t>
   </si>
   <si>
-    <t>0.15%</t>
-  </si>
-  <si>
     <t>[1360~1380)</t>
   </si>
   <si>
@@ -475,15 +367,9 @@
     <t>[2300~2320)</t>
   </si>
   <si>
-    <t>0.70%</t>
-  </si>
-  <si>
     <t>[2320~2340)</t>
   </si>
   <si>
-    <t>0.19%</t>
-  </si>
-  <si>
     <t>[2340~2360)</t>
   </si>
   <si>
@@ -544,9 +430,6 @@
     <t>[2760~2780)</t>
   </si>
   <si>
-    <t>0.84%</t>
-  </si>
-  <si>
     <t>[2780~2800)</t>
   </si>
   <si>
@@ -665,12 +548,24 @@
   </si>
   <si>
     <t>[4480~4500)</t>
+  </si>
+  <si>
+    <t>Total Requests</t>
+  </si>
+  <si>
+    <t>Max Delay Time/us</t>
+  </si>
+  <si>
+    <t>Top percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -708,9 +603,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,531 +1181,531 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$175</c:f>
+              <c:f>Sheet1!$D$2:$D$175</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="174"/>
                 <c:pt idx="0">
-                  <c:v>265</c:v>
+                  <c:v>5.590717299578059</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>149</c:v>
+                  <c:v>3.143459915611815</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>0.4641350210970464</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>0.3586497890295359</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>282</c:v>
+                  <c:v>5.949367088607595</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>665</c:v>
+                  <c:v>14.0295358649789</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>113</c:v>
+                  <c:v>2.383966244725738</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>225</c:v>
+                  <c:v>4.746835443037975</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>264</c:v>
+                  <c:v>5.569620253164556</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>359</c:v>
+                  <c:v>7.573839662447257</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>549</c:v>
+                  <c:v>11.58227848101266</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>334</c:v>
+                  <c:v>7.046413502109705</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>144</c:v>
+                  <c:v>3.037974683544304</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>79</c:v>
+                  <c:v>1.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>58</c:v>
+                  <c:v>1.223628691983123</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>65</c:v>
+                  <c:v>1.371308016877637</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42</c:v>
+                  <c:v>0.8860759493670887</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>85</c:v>
+                  <c:v>1.793248945147679</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>119</c:v>
+                  <c:v>2.510548523206751</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>120</c:v>
+                  <c:v>2.531645569620253</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>49</c:v>
+                  <c:v>1.033755274261603</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13</c:v>
+                  <c:v>0.2742616033755275</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10</c:v>
+                  <c:v>0.2109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>26</c:v>
+                  <c:v>0.5485232067510549</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>26</c:v>
+                  <c:v>0.5485232067510549</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8</c:v>
+                  <c:v>0.1687763713080169</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8</c:v>
+                  <c:v>0.1687763713080169</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10</c:v>
+                  <c:v>0.2109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>16</c:v>
+                  <c:v>0.3375527426160337</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13</c:v>
+                  <c:v>0.2742616033755275</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>20</c:v>
+                  <c:v>0.4219409282700421</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>20</c:v>
+                  <c:v>0.4219409282700421</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>21</c:v>
+                  <c:v>0.4430379746835443</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>13</c:v>
+                  <c:v>0.2742616033755275</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6</c:v>
+                  <c:v>0.1265822784810127</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>8</c:v>
+                  <c:v>0.1687763713080169</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>12</c:v>
+                  <c:v>0.2531645569620253</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6</c:v>
+                  <c:v>0.1265822784810127</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>7</c:v>
+                  <c:v>0.1476793248945148</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>6</c:v>
+                  <c:v>0.1265822784810127</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>8</c:v>
+                  <c:v>0.1687763713080169</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>6</c:v>
+                  <c:v>0.1265822784810127</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>33</c:v>
+                  <c:v>0.6962025316455696</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>9</c:v>
+                  <c:v>0.189873417721519</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>7</c:v>
+                  <c:v>0.1476793248945148</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>6</c:v>
+                  <c:v>0.1265822784810127</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>22</c:v>
+                  <c:v>0.4641350210970464</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>8</c:v>
+                  <c:v>0.1687763713080169</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>40</c:v>
+                  <c:v>0.8438818565400843</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>9</c:v>
+                  <c:v>0.189873417721519</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>8</c:v>
+                  <c:v>0.1687763713080169</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>10</c:v>
+                  <c:v>0.2109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>21</c:v>
+                  <c:v>0.4430379746835443</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>10</c:v>
+                  <c:v>0.2109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>6</c:v>
+                  <c:v>0.1265822784810127</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>5</c:v>
+                  <c:v>0.1054852320675105</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>3</c:v>
+                  <c:v>0.06329113924050633</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>4</c:v>
+                  <c:v>0.08438818565400844</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>2</c:v>
+                  <c:v>0.04219409282700422</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>1</c:v>
+                  <c:v>0.02109704641350211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1867,7 +1763,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Request Counts</a:t>
+                  <a:t>Percentage</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1901,13 +1797,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>65</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2215,13 +2111,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D175"/>
+  <dimension ref="A1:J175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2234,8 +2130,23 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2245,428 +2156,528 @@
       <c r="C2">
         <v>265</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="2">
+        <v>5.590717299578059</v>
+      </c>
+      <c r="F2">
+        <v>4740</v>
+      </c>
+      <c r="G2">
+        <v>4498</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2">
+        <v>14.0295358649789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>149</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" s="2">
+        <v>3.143459915611815</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2">
+        <v>11.58227848101266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="2">
+        <v>0.4641350210970464</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2">
+        <v>7.573839662447257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="2">
+        <v>0.3586497890295359</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7.046413502109705</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="2">
+        <v>0.04219409282700422</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5.949367088607595</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>282</v>
       </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="2">
+        <v>5.949367088607595</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5.590717299578059</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>665</v>
       </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="2">
+        <v>14.0295358649789</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5.569620253164556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>113</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="2">
+        <v>2.383966244725738</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4.746835443037975</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>225</v>
       </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" s="2">
+        <v>4.746835443037975</v>
+      </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2">
+        <v>3.143459915611815</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>264</v>
       </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="2">
+        <v>5.569620253164556</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3.037974683544304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>359</v>
       </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" s="2">
+        <v>7.573839662447257</v>
+      </c>
+      <c r="I12" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2.531645569620253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>549</v>
       </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" s="2">
+        <v>11.58227848101266</v>
+      </c>
+      <c r="I13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2.510548523206751</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>334</v>
       </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="2">
+        <v>7.046413502109705</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2.383966244725738</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>144</v>
       </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" s="2">
+        <v>3.037974683544304</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.793248945147679</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>79</v>
       </c>
-      <c r="D16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" s="2">
+        <v>1.666666666666667</v>
+      </c>
+      <c r="I16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.666666666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>58</v>
       </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="2">
+        <v>1.223628691983123</v>
+      </c>
+      <c r="J17">
+        <f>SUM(J2:J16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>65</v>
       </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" s="2">
+        <v>1.371308016877637</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>42</v>
       </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="2">
+        <v>0.8860759493670887</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>85</v>
       </c>
-      <c r="D20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="2">
+        <v>1.793248945147679</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>119</v>
       </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="2">
+        <v>2.510548523206751</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>120</v>
       </c>
-      <c r="D22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="2">
+        <v>2.531645569620253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>49</v>
       </c>
-      <c r="D23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="D23" s="2">
+        <v>1.033755274261603</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>13</v>
       </c>
-      <c r="D24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" s="2">
+        <v>0.2742616033755275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>10</v>
       </c>
-      <c r="D25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" s="2">
+        <v>0.2109704641350211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>26</v>
       </c>
-      <c r="D26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" s="2">
+        <v>0.5485232067510549</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>26</v>
       </c>
-      <c r="D27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="D27" s="2">
+        <v>0.5485232067510549</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>8</v>
       </c>
-      <c r="D28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28" s="2">
+        <v>0.1687763713080169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>8</v>
       </c>
-      <c r="D29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" s="2">
+        <v>0.1687763713080169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>10</v>
       </c>
-      <c r="D30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="D30" s="2">
+        <v>0.2109704641350211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C31">
         <v>16</v>
       </c>
-      <c r="D31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="D31" s="2">
+        <v>0.3375527426160337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
-      <c r="D32" t="s">
-        <v>13</v>
+      <c r="D32" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2674,13 +2685,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C33">
         <v>13</v>
       </c>
-      <c r="D33" t="s">
-        <v>49</v>
+      <c r="D33" s="2">
+        <v>0.2742616033755275</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2688,13 +2699,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
-      <c r="D34" t="s">
-        <v>13</v>
+      <c r="D34" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2702,13 +2713,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="C35">
         <v>5</v>
       </c>
-      <c r="D35" t="s">
-        <v>65</v>
+      <c r="D35" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2716,13 +2727,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C36">
         <v>20</v>
       </c>
-      <c r="D36" t="s">
-        <v>67</v>
+      <c r="D36" s="2">
+        <v>0.4219409282700421</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2730,13 +2741,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="C37">
         <v>4</v>
       </c>
-      <c r="D37" t="s">
-        <v>69</v>
+      <c r="D37" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2744,13 +2755,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
-      <c r="D38" t="s">
-        <v>71</v>
+      <c r="D38" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2758,13 +2769,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
-      <c r="D39" t="s">
-        <v>13</v>
+      <c r="D39" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2772,13 +2783,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C40">
         <v>20</v>
       </c>
-      <c r="D40" t="s">
-        <v>67</v>
+      <c r="D40" s="2">
+        <v>0.4219409282700421</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2786,13 +2797,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="C41">
         <v>21</v>
       </c>
-      <c r="D41" t="s">
-        <v>75</v>
+      <c r="D41" s="2">
+        <v>0.4430379746835443</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2800,13 +2811,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C42">
         <v>4</v>
       </c>
-      <c r="D42" t="s">
-        <v>69</v>
+      <c r="D42" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2814,13 +2825,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
-      <c r="D43" t="s">
-        <v>13</v>
+      <c r="D43" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2828,13 +2839,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="C44">
         <v>4</v>
       </c>
-      <c r="D44" t="s">
-        <v>69</v>
+      <c r="D44" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2842,13 +2853,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="C45">
         <v>13</v>
       </c>
-      <c r="D45" t="s">
-        <v>49</v>
+      <c r="D45" s="2">
+        <v>0.2742616033755275</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2856,13 +2867,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
-      <c r="D46" t="s">
-        <v>71</v>
+      <c r="D46" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2870,13 +2881,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="C47">
         <v>2</v>
       </c>
-      <c r="D47" t="s">
-        <v>13</v>
+      <c r="D47" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2884,13 +2895,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="C48">
         <v>6</v>
       </c>
-      <c r="D48" t="s">
-        <v>83</v>
+      <c r="D48" s="2">
+        <v>0.1265822784810127</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2898,13 +2909,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="C49">
         <v>3</v>
       </c>
-      <c r="D49" t="s">
-        <v>71</v>
+      <c r="D49" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2912,13 +2923,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="C50">
         <v>8</v>
       </c>
-      <c r="D50" t="s">
-        <v>56</v>
+      <c r="D50" s="2">
+        <v>0.1687763713080169</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2926,13 +2937,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="C51">
         <v>2</v>
       </c>
-      <c r="D51" t="s">
-        <v>13</v>
+      <c r="D51" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2940,13 +2951,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C52">
         <v>2</v>
       </c>
-      <c r="D52" t="s">
-        <v>13</v>
+      <c r="D52" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2954,13 +2965,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="C53">
         <v>2</v>
       </c>
-      <c r="D53" t="s">
-        <v>13</v>
+      <c r="D53" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2968,13 +2979,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="C54">
         <v>3</v>
       </c>
-      <c r="D54" t="s">
-        <v>71</v>
+      <c r="D54" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2982,13 +2993,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="C55">
         <v>4</v>
       </c>
-      <c r="D55" t="s">
-        <v>69</v>
+      <c r="D55" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2996,13 +3007,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
-      <c r="D56" t="s">
-        <v>92</v>
+      <c r="D56" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -3010,13 +3021,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="C57">
         <v>12</v>
       </c>
-      <c r="D57" t="s">
-        <v>94</v>
+      <c r="D57" s="2">
+        <v>0.2531645569620253</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -3024,13 +3035,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="C58">
         <v>5</v>
       </c>
-      <c r="D58" t="s">
-        <v>65</v>
+      <c r="D58" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -3038,13 +3049,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="C59">
         <v>3</v>
       </c>
-      <c r="D59" t="s">
-        <v>71</v>
+      <c r="D59" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -3052,13 +3063,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C60">
         <v>3</v>
       </c>
-      <c r="D60" t="s">
-        <v>71</v>
+      <c r="D60" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -3066,13 +3077,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="C61">
         <v>2</v>
       </c>
-      <c r="D61" t="s">
-        <v>13</v>
+      <c r="D61" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -3080,13 +3091,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="C62">
         <v>6</v>
       </c>
-      <c r="D62" t="s">
-        <v>83</v>
+      <c r="D62" s="2">
+        <v>0.1265822784810127</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -3094,13 +3105,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="C63">
         <v>4</v>
       </c>
-      <c r="D63" t="s">
-        <v>69</v>
+      <c r="D63" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -3108,13 +3119,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="C64">
         <v>2</v>
       </c>
-      <c r="D64" t="s">
-        <v>13</v>
+      <c r="D64" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -3122,13 +3133,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="C65">
         <v>2</v>
       </c>
-      <c r="D65" t="s">
-        <v>13</v>
+      <c r="D65" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -3136,13 +3147,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="C66">
         <v>2</v>
       </c>
-      <c r="D66" t="s">
-        <v>13</v>
+      <c r="D66" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -3150,13 +3161,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="C67">
         <v>3</v>
       </c>
-      <c r="D67" t="s">
-        <v>71</v>
+      <c r="D67" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -3164,13 +3175,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="C68">
         <v>3</v>
       </c>
-      <c r="D68" t="s">
-        <v>71</v>
+      <c r="D68" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -3178,13 +3189,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="C69">
         <v>7</v>
       </c>
-      <c r="D69" t="s">
-        <v>107</v>
+      <c r="D69" s="2">
+        <v>0.1476793248945148</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -3192,13 +3203,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="C70">
         <v>3</v>
       </c>
-      <c r="D70" t="s">
-        <v>71</v>
+      <c r="D70" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -3206,13 +3217,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="C71">
         <v>5</v>
       </c>
-      <c r="D71" t="s">
-        <v>65</v>
+      <c r="D71" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -3220,13 +3231,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="C72">
         <v>3</v>
       </c>
-      <c r="D72" t="s">
-        <v>71</v>
+      <c r="D72" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -3234,13 +3245,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
-      <c r="D73" t="s">
-        <v>92</v>
+      <c r="D73" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -3248,13 +3259,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="C74">
         <v>2</v>
       </c>
-      <c r="D74" t="s">
-        <v>13</v>
+      <c r="D74" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -3262,13 +3273,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="C75">
         <v>2</v>
       </c>
-      <c r="D75" t="s">
-        <v>13</v>
+      <c r="D75" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -3276,13 +3287,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="C76">
         <v>3</v>
       </c>
-      <c r="D76" t="s">
-        <v>71</v>
+      <c r="D76" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -3290,13 +3301,13 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="C77">
         <v>3</v>
       </c>
-      <c r="D77" t="s">
-        <v>71</v>
+      <c r="D77" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -3304,13 +3315,13 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="C78">
         <v>1</v>
       </c>
-      <c r="D78" t="s">
-        <v>92</v>
+      <c r="D78" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -3318,13 +3329,13 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="C79">
         <v>4</v>
       </c>
-      <c r="D79" t="s">
-        <v>69</v>
+      <c r="D79" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -3332,13 +3343,13 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="C80">
         <v>3</v>
       </c>
-      <c r="D80" t="s">
-        <v>71</v>
+      <c r="D80" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -3346,13 +3357,13 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="C81">
         <v>2</v>
       </c>
-      <c r="D81" t="s">
-        <v>13</v>
+      <c r="D81" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -3360,13 +3371,13 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C82">
         <v>3</v>
       </c>
-      <c r="D82" t="s">
-        <v>71</v>
+      <c r="D82" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -3374,13 +3385,13 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="C83">
         <v>3</v>
       </c>
-      <c r="D83" t="s">
-        <v>71</v>
+      <c r="D83" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -3388,13 +3399,13 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="C84">
         <v>2</v>
       </c>
-      <c r="D84" t="s">
-        <v>13</v>
+      <c r="D84" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -3402,13 +3413,13 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>123</v>
+        <v>87</v>
       </c>
       <c r="C85">
         <v>1</v>
       </c>
-      <c r="D85" t="s">
-        <v>92</v>
+      <c r="D85" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -3416,13 +3427,13 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>124</v>
+        <v>88</v>
       </c>
       <c r="C86">
         <v>5</v>
       </c>
-      <c r="D86" t="s">
-        <v>65</v>
+      <c r="D86" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -3430,13 +3441,13 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="C87">
         <v>2</v>
       </c>
-      <c r="D87" t="s">
-        <v>13</v>
+      <c r="D87" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -3444,13 +3455,13 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="C88">
         <v>2</v>
       </c>
-      <c r="D88" t="s">
-        <v>13</v>
+      <c r="D88" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -3458,13 +3469,13 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="C89">
         <v>2</v>
       </c>
-      <c r="D89" t="s">
-        <v>13</v>
+      <c r="D89" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -3472,13 +3483,13 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="C90">
         <v>2</v>
       </c>
-      <c r="D90" t="s">
-        <v>13</v>
+      <c r="D90" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -3486,13 +3497,13 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="C91">
         <v>4</v>
       </c>
-      <c r="D91" t="s">
-        <v>69</v>
+      <c r="D91" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -3500,13 +3511,13 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="C92">
         <v>3</v>
       </c>
-      <c r="D92" t="s">
-        <v>71</v>
+      <c r="D92" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -3514,13 +3525,13 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="C93">
         <v>3</v>
       </c>
-      <c r="D93" t="s">
-        <v>71</v>
+      <c r="D93" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -3528,13 +3539,13 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="C94">
         <v>5</v>
       </c>
-      <c r="D94" t="s">
-        <v>65</v>
+      <c r="D94" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -3542,13 +3553,13 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="C95">
         <v>2</v>
       </c>
-      <c r="D95" t="s">
-        <v>13</v>
+      <c r="D95" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -3556,13 +3567,13 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="C96">
         <v>6</v>
       </c>
-      <c r="D96" t="s">
-        <v>83</v>
+      <c r="D96" s="2">
+        <v>0.1265822784810127</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3570,13 +3581,13 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="C97">
         <v>3</v>
       </c>
-      <c r="D97" t="s">
-        <v>71</v>
+      <c r="D97" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3584,13 +3595,13 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="C98">
         <v>4</v>
       </c>
-      <c r="D98" t="s">
-        <v>69</v>
+      <c r="D98" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3598,13 +3609,13 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
-      <c r="D99" t="s">
-        <v>13</v>
+      <c r="D99" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -3612,13 +3623,13 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="C100">
         <v>8</v>
       </c>
-      <c r="D100" t="s">
-        <v>56</v>
+      <c r="D100" s="2">
+        <v>0.1687763713080169</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -3626,13 +3637,13 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
-      <c r="D101" t="s">
-        <v>13</v>
+      <c r="D101" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -3640,13 +3651,13 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>140</v>
+        <v>104</v>
       </c>
       <c r="C102">
         <v>2</v>
       </c>
-      <c r="D102" t="s">
-        <v>13</v>
+      <c r="D102" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3654,13 +3665,13 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C103">
         <v>2</v>
       </c>
-      <c r="D103" t="s">
-        <v>13</v>
+      <c r="D103" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3668,13 +3679,13 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="C104">
         <v>6</v>
       </c>
-      <c r="D104" t="s">
-        <v>83</v>
+      <c r="D104" s="2">
+        <v>0.1265822784810127</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3682,13 +3693,13 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>143</v>
+        <v>107</v>
       </c>
       <c r="C105">
         <v>2</v>
       </c>
-      <c r="D105" t="s">
-        <v>13</v>
+      <c r="D105" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -3696,13 +3707,13 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>144</v>
+        <v>108</v>
       </c>
       <c r="C106">
         <v>1</v>
       </c>
-      <c r="D106" t="s">
-        <v>92</v>
+      <c r="D106" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -3710,13 +3721,13 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="C107">
         <v>2</v>
       </c>
-      <c r="D107" t="s">
-        <v>13</v>
+      <c r="D107" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3724,13 +3735,13 @@
         <v>109</v>
       </c>
       <c r="B108" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="C108">
         <v>2</v>
       </c>
-      <c r="D108" t="s">
-        <v>13</v>
+      <c r="D108" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -3738,13 +3749,13 @@
         <v>110</v>
       </c>
       <c r="B109" t="s">
-        <v>147</v>
+        <v>111</v>
       </c>
       <c r="C109">
         <v>2</v>
       </c>
-      <c r="D109" t="s">
-        <v>13</v>
+      <c r="D109" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -3752,13 +3763,13 @@
         <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="C110">
         <v>2</v>
       </c>
-      <c r="D110" t="s">
-        <v>13</v>
+      <c r="D110" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -3766,13 +3777,13 @@
         <v>112</v>
       </c>
       <c r="B111" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="C111">
         <v>4</v>
       </c>
-      <c r="D111" t="s">
-        <v>69</v>
+      <c r="D111" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -3780,13 +3791,13 @@
         <v>113</v>
       </c>
       <c r="B112" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C112">
         <v>3</v>
       </c>
-      <c r="D112" t="s">
-        <v>71</v>
+      <c r="D112" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3794,13 +3805,13 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="C113">
         <v>1</v>
       </c>
-      <c r="D113" t="s">
-        <v>92</v>
+      <c r="D113" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3808,13 +3819,13 @@
         <v>115</v>
       </c>
       <c r="B114" t="s">
-        <v>152</v>
+        <v>116</v>
       </c>
       <c r="C114">
         <v>33</v>
       </c>
-      <c r="D114" t="s">
-        <v>153</v>
+      <c r="D114" s="2">
+        <v>0.6962025316455696</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3822,13 +3833,13 @@
         <v>116</v>
       </c>
       <c r="B115" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="C115">
         <v>9</v>
       </c>
-      <c r="D115" t="s">
-        <v>155</v>
+      <c r="D115" s="2">
+        <v>0.189873417721519</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3836,13 +3847,13 @@
         <v>117</v>
       </c>
       <c r="B116" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="C116">
         <v>3</v>
       </c>
-      <c r="D116" t="s">
-        <v>71</v>
+      <c r="D116" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3850,13 +3861,13 @@
         <v>118</v>
       </c>
       <c r="B117" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="C117">
         <v>4</v>
       </c>
-      <c r="D117" t="s">
-        <v>69</v>
+      <c r="D117" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3864,13 +3875,13 @@
         <v>120</v>
       </c>
       <c r="B118" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="C118">
         <v>7</v>
       </c>
-      <c r="D118" t="s">
-        <v>107</v>
+      <c r="D118" s="2">
+        <v>0.1476793248945148</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3878,13 +3889,13 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="C119">
         <v>6</v>
       </c>
-      <c r="D119" t="s">
-        <v>83</v>
+      <c r="D119" s="2">
+        <v>0.1265822784810127</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3892,13 +3903,13 @@
         <v>122</v>
       </c>
       <c r="B120" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="C120">
         <v>1</v>
       </c>
-      <c r="D120" t="s">
-        <v>92</v>
+      <c r="D120" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3906,13 +3917,13 @@
         <v>123</v>
       </c>
       <c r="B121" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
-      <c r="D121" t="s">
-        <v>13</v>
+      <c r="D121" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3920,13 +3931,13 @@
         <v>124</v>
       </c>
       <c r="B122" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="C122">
         <v>1</v>
       </c>
-      <c r="D122" t="s">
-        <v>92</v>
+      <c r="D122" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3934,13 +3945,13 @@
         <v>125</v>
       </c>
       <c r="B123" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="C123">
         <v>2</v>
       </c>
-      <c r="D123" t="s">
-        <v>13</v>
+      <c r="D123" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3948,13 +3959,13 @@
         <v>126</v>
       </c>
       <c r="B124" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
       <c r="C124">
         <v>3</v>
       </c>
-      <c r="D124" t="s">
-        <v>71</v>
+      <c r="D124" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3962,13 +3973,13 @@
         <v>127</v>
       </c>
       <c r="B125" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
-      <c r="D125" t="s">
-        <v>92</v>
+      <c r="D125" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3976,13 +3987,13 @@
         <v>129</v>
       </c>
       <c r="B126" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="C126">
         <v>1</v>
       </c>
-      <c r="D126" t="s">
-        <v>92</v>
+      <c r="D126" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3990,13 +4001,13 @@
         <v>130</v>
       </c>
       <c r="B127" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="C127">
         <v>1</v>
       </c>
-      <c r="D127" t="s">
-        <v>92</v>
+      <c r="D127" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -4004,13 +4015,13 @@
         <v>131</v>
       </c>
       <c r="B128" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="C128">
         <v>2</v>
       </c>
-      <c r="D128" t="s">
-        <v>13</v>
+      <c r="D128" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -4018,13 +4029,13 @@
         <v>132</v>
       </c>
       <c r="B129" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="C129">
         <v>1</v>
       </c>
-      <c r="D129" t="s">
-        <v>92</v>
+      <c r="D129" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -4032,13 +4043,13 @@
         <v>133</v>
       </c>
       <c r="B130" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="C130">
         <v>22</v>
       </c>
-      <c r="D130" t="s">
-        <v>9</v>
+      <c r="D130" s="2">
+        <v>0.4641350210970464</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -4046,13 +4057,13 @@
         <v>134</v>
       </c>
       <c r="B131" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="C131">
         <v>5</v>
       </c>
-      <c r="D131" t="s">
-        <v>65</v>
+      <c r="D131" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -4060,13 +4071,13 @@
         <v>135</v>
       </c>
       <c r="B132" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="C132">
         <v>1</v>
       </c>
-      <c r="D132" t="s">
-        <v>92</v>
+      <c r="D132" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -4074,13 +4085,13 @@
         <v>136</v>
       </c>
       <c r="B133" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="C133">
         <v>2</v>
       </c>
-      <c r="D133" t="s">
-        <v>13</v>
+      <c r="D133" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -4088,13 +4099,13 @@
         <v>137</v>
       </c>
       <c r="B134" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="C134">
         <v>8</v>
       </c>
-      <c r="D134" t="s">
-        <v>56</v>
+      <c r="D134" s="2">
+        <v>0.1687763713080169</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -4102,13 +4113,13 @@
         <v>138</v>
       </c>
       <c r="B135" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="C135">
         <v>40</v>
       </c>
-      <c r="D135" t="s">
-        <v>176</v>
+      <c r="D135" s="2">
+        <v>0.8438818565400843</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -4116,13 +4127,13 @@
         <v>139</v>
       </c>
       <c r="B136" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
       <c r="C136">
         <v>9</v>
       </c>
-      <c r="D136" t="s">
-        <v>155</v>
+      <c r="D136" s="2">
+        <v>0.189873417721519</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -4130,13 +4141,13 @@
         <v>140</v>
       </c>
       <c r="B137" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="C137">
         <v>8</v>
       </c>
-      <c r="D137" t="s">
-        <v>56</v>
+      <c r="D137" s="2">
+        <v>0.1687763713080169</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -4144,13 +4155,13 @@
         <v>141</v>
       </c>
       <c r="B138" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="C138">
         <v>2</v>
       </c>
-      <c r="D138" t="s">
-        <v>13</v>
+      <c r="D138" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -4158,13 +4169,13 @@
         <v>142</v>
       </c>
       <c r="B139" t="s">
-        <v>180</v>
+        <v>141</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
-      <c r="D139" t="s">
-        <v>92</v>
+      <c r="D139" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -4172,13 +4183,13 @@
         <v>143</v>
       </c>
       <c r="B140" t="s">
-        <v>181</v>
+        <v>142</v>
       </c>
       <c r="C140">
         <v>1</v>
       </c>
-      <c r="D140" t="s">
-        <v>92</v>
+      <c r="D140" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -4186,13 +4197,13 @@
         <v>145</v>
       </c>
       <c r="B141" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="C141">
         <v>1</v>
       </c>
-      <c r="D141" t="s">
-        <v>92</v>
+      <c r="D141" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -4200,13 +4211,13 @@
         <v>147</v>
       </c>
       <c r="B142" t="s">
-        <v>183</v>
+        <v>144</v>
       </c>
       <c r="C142">
         <v>1</v>
       </c>
-      <c r="D142" t="s">
-        <v>92</v>
+      <c r="D142" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -4214,13 +4225,13 @@
         <v>149</v>
       </c>
       <c r="B143" t="s">
-        <v>184</v>
+        <v>145</v>
       </c>
       <c r="C143">
         <v>10</v>
       </c>
-      <c r="D143" t="s">
-        <v>51</v>
+      <c r="D143" s="2">
+        <v>0.2109704641350211</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -4228,13 +4239,13 @@
         <v>150</v>
       </c>
       <c r="B144" t="s">
-        <v>185</v>
+        <v>146</v>
       </c>
       <c r="C144">
         <v>4</v>
       </c>
-      <c r="D144" t="s">
-        <v>69</v>
+      <c r="D144" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -4242,13 +4253,13 @@
         <v>152</v>
       </c>
       <c r="B145" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="C145">
         <v>1</v>
       </c>
-      <c r="D145" t="s">
-        <v>92</v>
+      <c r="D145" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -4256,13 +4267,13 @@
         <v>153</v>
       </c>
       <c r="B146" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="C146">
         <v>2</v>
       </c>
-      <c r="D146" t="s">
-        <v>13</v>
+      <c r="D146" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -4270,13 +4281,13 @@
         <v>155</v>
       </c>
       <c r="B147" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="C147">
         <v>21</v>
       </c>
-      <c r="D147" t="s">
-        <v>75</v>
+      <c r="D147" s="2">
+        <v>0.4430379746835443</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -4284,13 +4295,13 @@
         <v>156</v>
       </c>
       <c r="B148" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="C148">
         <v>5</v>
       </c>
-      <c r="D148" t="s">
-        <v>65</v>
+      <c r="D148" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -4298,13 +4309,13 @@
         <v>157</v>
       </c>
       <c r="B149" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="C149">
         <v>5</v>
       </c>
-      <c r="D149" t="s">
-        <v>65</v>
+      <c r="D149" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -4312,13 +4323,13 @@
         <v>158</v>
       </c>
       <c r="B150" t="s">
-        <v>191</v>
+        <v>152</v>
       </c>
       <c r="C150">
         <v>10</v>
       </c>
-      <c r="D150" t="s">
-        <v>51</v>
+      <c r="D150" s="2">
+        <v>0.2109704641350211</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -4326,13 +4337,13 @@
         <v>160</v>
       </c>
       <c r="B151" t="s">
-        <v>192</v>
+        <v>153</v>
       </c>
       <c r="C151">
         <v>5</v>
       </c>
-      <c r="D151" t="s">
-        <v>65</v>
+      <c r="D151" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -4340,13 +4351,13 @@
         <v>161</v>
       </c>
       <c r="B152" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="C152">
         <v>1</v>
       </c>
-      <c r="D152" t="s">
-        <v>92</v>
+      <c r="D152" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -4354,13 +4365,13 @@
         <v>162</v>
       </c>
       <c r="B153" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
       <c r="C153">
         <v>6</v>
       </c>
-      <c r="D153" t="s">
-        <v>83</v>
+      <c r="D153" s="2">
+        <v>0.1265822784810127</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -4368,13 +4379,13 @@
         <v>163</v>
       </c>
       <c r="B154" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="C154">
         <v>3</v>
       </c>
-      <c r="D154" t="s">
-        <v>71</v>
+      <c r="D154" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -4382,13 +4393,13 @@
         <v>164</v>
       </c>
       <c r="B155" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="C155">
         <v>2</v>
       </c>
-      <c r="D155" t="s">
-        <v>13</v>
+      <c r="D155" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -4396,13 +4407,13 @@
         <v>167</v>
       </c>
       <c r="B156" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="C156">
         <v>1</v>
       </c>
-      <c r="D156" t="s">
-        <v>92</v>
+      <c r="D156" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -4410,13 +4421,13 @@
         <v>171</v>
       </c>
       <c r="B157" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="C157">
         <v>1</v>
       </c>
-      <c r="D157" t="s">
-        <v>92</v>
+      <c r="D157" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -4424,13 +4435,13 @@
         <v>172</v>
       </c>
       <c r="B158" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="C158">
         <v>5</v>
       </c>
-      <c r="D158" t="s">
-        <v>65</v>
+      <c r="D158" s="2">
+        <v>0.1054852320675105</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -4438,13 +4449,13 @@
         <v>173</v>
       </c>
       <c r="B159" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="C159">
         <v>1</v>
       </c>
-      <c r="D159" t="s">
-        <v>92</v>
+      <c r="D159" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -4452,13 +4463,13 @@
         <v>174</v>
       </c>
       <c r="B160" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="C160">
         <v>3</v>
       </c>
-      <c r="D160" t="s">
-        <v>71</v>
+      <c r="D160" s="2">
+        <v>0.06329113924050633</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -4466,13 +4477,13 @@
         <v>177</v>
       </c>
       <c r="B161" t="s">
-        <v>202</v>
+        <v>163</v>
       </c>
       <c r="C161">
         <v>1</v>
       </c>
-      <c r="D161" t="s">
-        <v>92</v>
+      <c r="D161" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4480,13 +4491,13 @@
         <v>178</v>
       </c>
       <c r="B162" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="C162">
         <v>1</v>
       </c>
-      <c r="D162" t="s">
-        <v>92</v>
+      <c r="D162" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -4494,13 +4505,13 @@
         <v>181</v>
       </c>
       <c r="B163" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
       <c r="C163">
         <v>4</v>
       </c>
-      <c r="D163" t="s">
-        <v>69</v>
+      <c r="D163" s="2">
+        <v>0.08438818565400844</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -4508,13 +4519,13 @@
         <v>186</v>
       </c>
       <c r="B164" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="C164">
         <v>1</v>
       </c>
-      <c r="D164" t="s">
-        <v>92</v>
+      <c r="D164" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -4522,13 +4533,13 @@
         <v>187</v>
       </c>
       <c r="B165" t="s">
-        <v>206</v>
+        <v>167</v>
       </c>
       <c r="C165">
         <v>2</v>
       </c>
-      <c r="D165" t="s">
-        <v>13</v>
+      <c r="D165" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -4536,13 +4547,13 @@
         <v>189</v>
       </c>
       <c r="B166" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="C166">
         <v>1</v>
       </c>
-      <c r="D166" t="s">
-        <v>92</v>
+      <c r="D166" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -4550,13 +4561,13 @@
         <v>191</v>
       </c>
       <c r="B167" t="s">
-        <v>208</v>
+        <v>169</v>
       </c>
       <c r="C167">
         <v>1</v>
       </c>
-      <c r="D167" t="s">
-        <v>92</v>
+      <c r="D167" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4564,13 +4575,13 @@
         <v>193</v>
       </c>
       <c r="B168" t="s">
-        <v>209</v>
+        <v>170</v>
       </c>
       <c r="C168">
         <v>2</v>
       </c>
-      <c r="D168" t="s">
-        <v>13</v>
+      <c r="D168" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4578,13 +4589,13 @@
         <v>195</v>
       </c>
       <c r="B169" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="C169">
         <v>2</v>
       </c>
-      <c r="D169" t="s">
-        <v>13</v>
+      <c r="D169" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -4592,13 +4603,13 @@
         <v>196</v>
       </c>
       <c r="B170" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="C170">
         <v>1</v>
       </c>
-      <c r="D170" t="s">
-        <v>92</v>
+      <c r="D170" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -4606,13 +4617,13 @@
         <v>203</v>
       </c>
       <c r="B171" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="C171">
         <v>1</v>
       </c>
-      <c r="D171" t="s">
-        <v>92</v>
+      <c r="D171" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -4620,13 +4631,13 @@
         <v>213</v>
       </c>
       <c r="B172" t="s">
-        <v>213</v>
+        <v>174</v>
       </c>
       <c r="C172">
         <v>1</v>
       </c>
-      <c r="D172" t="s">
-        <v>92</v>
+      <c r="D172" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -4634,13 +4645,13 @@
         <v>214</v>
       </c>
       <c r="B173" t="s">
-        <v>214</v>
+        <v>175</v>
       </c>
       <c r="C173">
         <v>2</v>
       </c>
-      <c r="D173" t="s">
-        <v>13</v>
+      <c r="D173" s="2">
+        <v>0.04219409282700422</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -4648,13 +4659,13 @@
         <v>221</v>
       </c>
       <c r="B174" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="C174">
         <v>1</v>
       </c>
-      <c r="D174" t="s">
-        <v>92</v>
+      <c r="D174" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4662,13 +4673,13 @@
         <v>224</v>
       </c>
       <c r="B175" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="C175">
         <v>1</v>
       </c>
-      <c r="D175" t="s">
-        <v>92</v>
+      <c r="D175" s="2">
+        <v>0.02109704641350211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>